<commit_message>
Update to work with noew changes for support for resw files on windows
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionExample/MultilingualExtensionExample/Resources/AppResources.nb-NO.resx.xlsx
+++ b/src/Samples/MultilingualExtensionExample/MultilingualExtensionExample/Resources/AppResources.nb-NO.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube er fint for videoer og musikk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snake</t>
   </si>
 </sst>
 </file>
@@ -163,6 +172,36 @@
       </c>
       <c r="E4"/>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fix for No Translation
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionExample/MultilingualExtensionExample/Resources/AppResources.nb-NO.resx.xlsx
+++ b/src/Samples/MultilingualExtensionExample/MultilingualExtensionExample/Resources/AppResources.nb-NO.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -26,16 +26,58 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">CSharp_Is_Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSharp is love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSharp er kjærlighet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App_Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enter_Your_Email</t>
   </si>
   <si>
     <t xml:space="preserve">Enter your email please</t>
   </si>
   <si>
-    <t xml:space="preserve">Skriv inn e-posten din, vennligst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need review</t>
+    <t xml:space="preserve">Skriv inn e-postadressen din</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter_Your_Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter your password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skriv inn passordet ditt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter_Your_Cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter your cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skriv inn katten din</t>
   </si>
   <si>
     <t xml:space="preserve">How_Old_Are_You</t>
@@ -59,10 +101,25 @@
     <t xml:space="preserve">Dog</t>
   </si>
   <si>
-    <t xml:space="preserve">New</t>
+    <t xml:space="preserve">Hund</t>
   </si>
   <si>
     <t xml:space="preserve">Snake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katt</t>
   </si>
 </sst>
 </file>
@@ -162,10 +219,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -174,16 +231,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5"/>
     </row>
@@ -192,15 +249,120 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>